<commit_message>
test cases document and bugs updated
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -5,13 +5,13 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - Bugs bunny report" sheetId="1" r:id="rId4"/>
+    <sheet name="Bugs bunny report" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Bugs bunny report</t>
   </si>
@@ -26,6 +26,12 @@
   </si>
   <si>
     <t>Steps to reproduce</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Observed Results</t>
   </si>
   <si>
     <t>Environment</t>
@@ -74,6 +80,12 @@
     </r>
   </si>
   <si>
+    <t>Products are sorted by actual price in ascending/descending order depending on user selection</t>
+  </si>
+  <si>
+    <t>Products are order with the original price, before discounts</t>
+  </si>
+  <si>
     <t xml:space="preserve"> - Firefox 82.0 / macOS 10.15
  - Chrome 86.0.4240.183 / macOS 10.15.7</t>
   </si>
@@ -85,6 +97,37 @@
   </si>
   <si>
     <t>FL-2</t>
+  </si>
+  <si>
+    <t>Google + url is different than expected</t>
+  </si>
+  <si>
+    <t>After clicking google+ logo, it goes to a redirect login from google that does not contains the original group</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Click on google+ icon on the bottom of the site
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Verify the actual URL</t>
+    </r>
+  </si>
+  <si>
+    <t>Url contains a redirect to original Gogole plus group</t>
+  </si>
+  <si>
+    <t>URL does not contain original path</t>
   </si>
   <si>
     <t>FL-3</t>
@@ -97,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -109,13 +152,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,12 +178,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="17"/>
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -147,6 +201,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -160,7 +236,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -169,7 +245,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -178,43 +254,43 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -223,28 +299,200 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -254,80 +502,97 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="ff000000"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="12"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="ff000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="12"/>
-          <bgColor indexed="14"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="ff000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="12"/>
+          <fgColor indexed="14"/>
           <bgColor indexed="15"/>
         </patternFill>
       </fill>
@@ -338,8 +603,74 @@
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="12"/>
+          <fgColor indexed="14"/>
           <bgColor indexed="16"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="ff000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="17"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="ff000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="ff000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="20"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="ff000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="21"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="ff000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="ff000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="23"/>
         </patternFill>
       </fill>
     </dxf>
@@ -356,15 +687,21 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="00000000"/>
+      <rgbColor rgb="ffafe489"/>
+      <rgbColor rgb="ffff9781"/>
+      <rgbColor rgb="fffffc98"/>
+      <rgbColor rgb="ff88ccff"/>
+      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="e5afe489"/>
       <rgbColor rgb="e5ff9781"/>
       <rgbColor rgb="e5fffc98"/>
       <rgbColor rgb="e588ccff"/>
-      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -381,10 +718,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -561,11 +898,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -574,34 +914,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -849,12 +1189,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1145,7 +1485,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1423,18 +1763,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:J32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.0156" style="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7812" style="1" customWidth="1"/>
-    <col min="4" max="4" width="47.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52" style="1" customWidth="1"/>
+    <col min="3" max="3" width="53.8516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="47.3516" style="1" customWidth="1"/>
     <col min="5" max="10" width="16.3516" style="1" customWidth="1"/>
     <col min="11" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
@@ -1443,439 +1781,481 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="H2" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s" s="5">
+        <v>9</v>
+      </c>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" ht="80.25" customHeight="1">
-      <c r="A3" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s" s="6">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s" s="7">
+      <c r="A3" t="s" s="8">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="B3" t="s" s="9">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="7">
+      <c r="C3" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="F3" t="s" s="7">
+      <c r="D3" t="s" s="11">
         <v>13</v>
       </c>
-      <c r="G3" t="s" s="7">
+      <c r="E3" t="s" s="11">
         <v>14</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="9">
+      <c r="F3" t="s" s="11">
         <v>15</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="G3" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s" s="13">
+        <v>18</v>
+      </c>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" ht="74.7" customHeight="1">
+      <c r="A4" t="s" s="15">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s" s="11">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s" s="16">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s" s="11">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s" s="11">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s" s="11">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s" s="17">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s" s="18">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s" s="19">
+        <v>18</v>
+      </c>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="A5" t="s" s="21">
+        <v>25</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="12"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="12"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="12"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="12"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="12"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="12"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="12"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" s="12"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
     </row>
     <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" s="12"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
     </row>
     <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" s="12"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" s="12"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" s="12"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G2:G32">
+  <conditionalFormatting sqref="I2:I3 G5:G32">
     <cfRule type="containsText" dxfId="0" priority="1" stopIfTrue="1" text="pass">
-      <formula>NOT(ISERROR(FIND(UPPER("pass"),UPPER(G2))))</formula>
+      <formula>NOT(ISERROR(FIND(UPPER("pass"),UPPER(I2))))</formula>
       <formula>"pass"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" stopIfTrue="1" text="fail">
-      <formula>NOT(ISERROR(FIND(UPPER("fail"),UPPER(G2))))</formula>
+      <formula>NOT(ISERROR(FIND(UPPER("fail"),UPPER(I2))))</formula>
       <formula>"fail"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="3" stopIfTrue="1" text="retest">
-      <formula>NOT(ISERROR(FIND(UPPER("retest"),UPPER(G2))))</formula>
+      <formula>NOT(ISERROR(FIND(UPPER("retest"),UPPER(I2))))</formula>
       <formula>"retest"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" text="fixed">
-      <formula>NOT(ISERROR(FIND(UPPER("fixed"),UPPER(G2))))</formula>
+      <formula>NOT(ISERROR(FIND(UPPER("fixed"),UPPER(I2))))</formula>
+      <formula>"fixed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="containsText" dxfId="4" priority="1" stopIfTrue="1" text="pass">
+      <formula>NOT(ISERROR(FIND(UPPER("pass"),UPPER(I4))))</formula>
+      <formula>"pass"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" text="fail">
+      <formula>NOT(ISERROR(FIND(UPPER("fail"),UPPER(I4))))</formula>
+      <formula>"fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="3" stopIfTrue="1" text="retest">
+      <formula>NOT(ISERROR(FIND(UPPER("retest"),UPPER(I4))))</formula>
+      <formula>"retest"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="4" stopIfTrue="1" text="fixed">
+      <formula>NOT(ISERROR(FIND(UPPER("fixed"),UPPER(I4))))</formula>
       <formula>"fixed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>